<commit_message>
Added search page home page script. Optimized POM classes by inheriting AbstractComponents class.
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/resources/metaPractise.xlsx
+++ b/src/main/java/com/test/resources/metaPractise.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15710" windowHeight="2700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15710" windowHeight="3040"/>
   </bookViews>
   <sheets>
     <sheet name="metaContent" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="161">
   <si>
     <t>Domain</t>
   </si>
@@ -118,72 +118,9 @@
     <t>Your next career move awaits in our General Listings. Explore diverse job opportunities at CompanyName in City, State</t>
   </si>
   <si>
-    <t>epicareerz.com</t>
-  </si>
-  <si>
-    <t>Your Next Career Move Begins Here | Home</t>
-  </si>
-  <si>
-    <t>Unlock the door to career advancement with our job board. Your journey starts here, connecting you with opportunities tailored to your goals</t>
-  </si>
-  <si>
-    <t>Effortless Job Discovery with Our Advanced Search</t>
-  </si>
-  <si>
-    <t>Discover the power of precision in your job search with us. Find, filter, and apply seamlessly to unlock a world of career possibilities.</t>
-  </si>
-  <si>
-    <t>Building Futures: Explore Our Job Board About Us</t>
-  </si>
-  <si>
-    <t>Discover the driving force behind. Learn about our history, values, and the vision that shapes our mission in the world of job opportunities.</t>
-  </si>
-  <si>
-    <t>Connect with Our Team: Contact Information</t>
-  </si>
-  <si>
-    <t>Customer support at your service. Contact Us for prompt assistance and guidance on navigating the platform and advancing your career.</t>
-  </si>
-  <si>
-    <t>Your Confidentiality Matters: Our Privacy Principles</t>
-  </si>
-  <si>
-    <t>Trust and security are paramount. Our Privacy Policy reveals the safeguards and commitments we have in place to protect your privacy and data.</t>
-  </si>
-  <si>
-    <t>Clear Guidelines: Our Terms &amp; Conditions Explained</t>
-  </si>
-  <si>
-    <t>Understanding the rules of engagement. Our Terms &amp; Conditions outline the responsibilities and opportunities that shape your path to career success.</t>
-  </si>
-  <si>
-    <t>Build Your Career with Top Companies - Our Job Listings</t>
-  </si>
-  <si>
-    <t>Build your career with top companies. Explore our employment opportunities and find the perfect job match that aligns with your skills and aspirations.</t>
-  </si>
-  <si>
-    <t>Explore Jobs in Nearby Locations with us</t>
-  </si>
-  <si>
-    <t>Unlock local job opportunities with us. Explore job listings in specific locations to find the perfect match for your skills and aspirations.</t>
-  </si>
-  <si>
-    <t>Diverse Careers at CompanyName in City, State</t>
-  </si>
-  <si>
-    <t>Navigate the realm of job possibilities with our General Listings at CompanyName in City, State.</t>
-  </si>
-  <si>
     <t>Cookie Policy</t>
   </si>
   <si>
-    <t>Your Choices, Our Cookies: Cookie Policy Overview</t>
-  </si>
-  <si>
-    <t>Navigate online interactions with confidence. Our Cookie Policy ensures transparency in how we utilize and enhance your user experience.</t>
-  </si>
-  <si>
     <t>jobzsphere.com</t>
   </si>
   <si>
@@ -377,6 +314,195 @@
   </si>
   <si>
     <t>Your career journey deserves transparency. Dive into our Cookie Policy to understand how we prioritize your digital well-being.</t>
+  </si>
+  <si>
+    <t>jobzfyi.com</t>
+  </si>
+  <si>
+    <t>Connecting Talent to Tomorrow's Opportunities Now</t>
+  </si>
+  <si>
+    <t>Connecting talent with opportunity - that's our mission. Explore the dynamic features of our home page and let your dream job find you.</t>
+  </si>
+  <si>
+    <t>Refine Your Job Search Effortlessly | Search Page</t>
+  </si>
+  <si>
+    <t>Navigate your job search journey with precision on our search page. Discover opportunities, filter results, and tailor your job hunt.</t>
+  </si>
+  <si>
+    <t>Connecting Talent with Opportunity - About Us</t>
+  </si>
+  <si>
+    <t>Connecting talent with opportunity is more than a tagline. Explore our About Us page to understand our mission, values, and the commitment we have.</t>
+  </si>
+  <si>
+    <t>Your Success Starts with Us - Contact Today</t>
+  </si>
+  <si>
+    <t>Together, we strive to develop an integrated job search platform that links job seekers with prominent organizations, fostering a smooth and effective connection</t>
+  </si>
+  <si>
+    <t>Your Information, Your Security - Privacy Policy</t>
+  </si>
+  <si>
+    <t>Unveil the privacy standards. Our Privacy Policy is your guide to understanding how we handle, protect, and respect your personal information.</t>
+  </si>
+  <si>
+    <t>Read Our Terms &amp; Conditions for Seamless Job Searches</t>
+  </si>
+  <si>
+    <t>Our Terms &amp; Conditions offer insights into the expectations, rights, and responsibilities that define your experience on our platform.</t>
+  </si>
+  <si>
+    <t>Your Next Professional Adventure Awaits - Company Careers</t>
+  </si>
+  <si>
+    <t>Advance your career with our  Company Jobs. Explore opportunities with reputable organizations committed to your professional growth and success.</t>
+  </si>
+  <si>
+    <t>Localize Your Career Journey - Location Based Jobs</t>
+  </si>
+  <si>
+    <t>Explore our Location Jobs that match your expertise and are located in your preferred geographical area.</t>
+  </si>
+  <si>
+    <t>Find Your Fit at CompanyName in City, State</t>
+  </si>
+  <si>
+    <t>Listings offer in-depth insights into various job positions at CompanyName in City, State allowing you to make informed career decisions.</t>
+  </si>
+  <si>
+    <t>Your Cookie Preferences Matter - Understanding Cookie</t>
+  </si>
+  <si>
+    <t>Your career path deserves a side of transparency. Delve into our Cookie Policy to see how we prioritize your digital well-being.</t>
+  </si>
+  <si>
+    <t>EmployRadar.com</t>
+  </si>
+  <si>
+    <t>Start Your Job Search Today | Your Home Page</t>
+  </si>
+  <si>
+    <t>Transform your career aspirations into reality. Begin your job search adventure on our home page, where opportunities meet ambition.</t>
+  </si>
+  <si>
+    <t>Fine-Tune Your Job Hunt | Advanced Search Filters</t>
+  </si>
+  <si>
+    <t>Discover the power of targeted job hunting on our search page. Your dream job is just a search away, with filters that align with your goals.</t>
+  </si>
+  <si>
+    <t>Unveiling Our Mission: Learn About Us</t>
+  </si>
+  <si>
+    <t>Uncover the driving force behind our job board by exploring our About Us page. Learn how we're shaping the future of careers with passion and purpose.</t>
+  </si>
+  <si>
+    <t>Let's Talk Careers: Contact Our Team Today</t>
+  </si>
+  <si>
+    <t>Connect with us directly through our Contact Us page. Your questions and concerns are important to us, and we're here to ensure a smooth career journey.</t>
+  </si>
+  <si>
+    <t>Trustworthy Practices: Our Privacy Standards</t>
+  </si>
+  <si>
+    <t>Explore the details of our Privacy Policy to understand how we prioritize the confidentiality and security of your information throughout your job search.</t>
+  </si>
+  <si>
+    <t>Your Commitment: Our Commitment, Our Terms</t>
+  </si>
+  <si>
+    <t>Explore our Terms &amp; Conditions to familiarize yourself with the rules governing your engagement with our job board, ensuring a smooth journey.</t>
+  </si>
+  <si>
+    <t>Unlock Potential: Our Company Job Listings</t>
+  </si>
+  <si>
+    <t>Connect with your dream company by exploring tailored job opportunities on our Company Jobs page. Your next career chapter begins here.</t>
+  </si>
+  <si>
+    <t>Connect with Local Employers: Location Jobs Nearby</t>
+  </si>
+  <si>
+    <t>Explore career opportunities in your desired locations on our Location Jobs page tailored to specific regions and uncover the perfect match.</t>
+  </si>
+  <si>
+    <t>All-in-One Job Hub at CompanyName in City, State</t>
+  </si>
+  <si>
+    <t>Explore the richness of career options on our General Listings Page at CompanyName in City, State from entry-level to executive roles.</t>
+  </si>
+  <si>
+    <t>Your Privacy, Our Cookies: Our Cookie Policy</t>
+  </si>
+  <si>
+    <t>Dive into our Cookie Policy to understand how we use cookies to provide you with a seamless and personalized job search journey.</t>
+  </si>
+  <si>
+    <t>medichirings.com</t>
+  </si>
+  <si>
+    <t>Embark on a career exploration journey by landing on our home page. Uncover a wealth of job opportunities tailored to your aspirations.</t>
+  </si>
+  <si>
+    <t>Filter, Find, Flourish: Our Job Board Search Options</t>
+  </si>
+  <si>
+    <t>Transform your job search into an efficient and personalized experience. Our search page is designed to connect you with the opportunities that matter.</t>
+  </si>
+  <si>
+    <t>Crafting Success Stories - Explore About Us</t>
+  </si>
+  <si>
+    <t>Embark on a journey of understanding our job board's ethos. Our About Us page delves into the core values that shape our commitment to your success.</t>
+  </si>
+  <si>
+    <t>Connect with Us: We Value Your Feedback</t>
+  </si>
+  <si>
+    <t>Explore the various ways to reach out to us on our Contact Us page. Your feedback and inquiries are valuable, and we're committed to assisting you.</t>
+  </si>
+  <si>
+    <t>Your Data, Your Rules: Explore Privacy Policy</t>
+  </si>
+  <si>
+    <t>Discover the measures we take to protect your privacy on our job board. Our Privacy Policy is a testament to our commitment to security.</t>
+  </si>
+  <si>
+    <t>Setting the Standard: Our Terms of Use</t>
+  </si>
+  <si>
+    <t>Discover the guidelines that define your experience on our job board. Our Terms &amp; Conditions provide the framework for a transparent career exploration.</t>
+  </si>
+  <si>
+    <t>Experience Growth: Top Company Career Options</t>
+  </si>
+  <si>
+    <t>Navigate through exclusive job listings tied to specific companies on our Company Jobs page. Your next career breakthrough could be just a click away.</t>
+  </si>
+  <si>
+    <t>Unlock Local Opportunities: Jobs by Location</t>
+  </si>
+  <si>
+    <t>Navigate through location-specific job listings on our Location Jobs page. Your ideal career move – explore and seize the opportunity.</t>
+  </si>
+  <si>
+    <t>Entry to Executive at CompanyName in City, State</t>
+  </si>
+  <si>
+    <t>Unlock a vast array of career possibilities with CompanyName in City, State. Tailor your search and find the job that perfectly aligns.</t>
+  </si>
+  <si>
+    <t>Optimize Your Experience: Our Cookie Practices</t>
+  </si>
+  <si>
+    <t>Navigate through our Cookie Policy to understand the importance of cookies in optimizing your experience on our job board.</t>
+  </si>
+  <si>
+    <t>Find Your Ideal Job Today - Where Careers Begin</t>
   </si>
 </sst>
 </file>
@@ -442,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -456,6 +582,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -739,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -796,7 +925,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -878,503 +1007,750 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>32</v>
+      <c r="A12" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>34</v>
+      <c r="C12" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
+      <c r="C13" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>38</v>
+      <c r="C14" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>40</v>
+      <c r="C15" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>42</v>
+      <c r="C16" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>44</v>
+      <c r="C17" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>46</v>
+      <c r="C18" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>48</v>
+      <c r="C19" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>50</v>
+      <c r="C20" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="3"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>53</v>
+        <v>32</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
-        <v>54</v>
+      <c r="A23" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="7"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="7"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="7"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="7"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="7"/>
+      <c r="A28" s="8"/>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="7"/>
+      <c r="A29" s="8"/>
       <c r="B29" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="7"/>
+      <c r="A30" s="8"/>
       <c r="B30" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="7"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="7"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="4" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="7" t="s">
-        <v>75</v>
+      <c r="A34" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="7"/>
+      <c r="A35" s="8"/>
       <c r="B35" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="7"/>
+      <c r="A36" s="8"/>
       <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="7"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="7"/>
+      <c r="A38" s="8"/>
       <c r="B38" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="7"/>
+      <c r="A39" s="8"/>
       <c r="B39" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="7"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="7"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="7"/>
+      <c r="A42" s="8"/>
       <c r="B42" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="7"/>
+      <c r="A43" s="8"/>
       <c r="B43" s="4" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="7" t="s">
-        <v>98</v>
+      <c r="A45" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="7"/>
+      <c r="A46" s="8"/>
       <c r="B46" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="7"/>
+      <c r="A47" s="8"/>
       <c r="B47" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="7"/>
+      <c r="A48" s="8"/>
       <c r="B48" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="7"/>
+      <c r="A49" s="8"/>
       <c r="B49" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="7"/>
+      <c r="A50" s="8"/>
       <c r="B50" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="7"/>
+      <c r="A51" s="8"/>
       <c r="B51" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="7"/>
+      <c r="A52" s="8"/>
       <c r="B52" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="7"/>
+      <c r="A53" s="8"/>
       <c r="B53" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="8"/>
+      <c r="B54" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="8"/>
+      <c r="B57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="8"/>
+      <c r="B58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="8"/>
+      <c r="B59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="8"/>
+      <c r="B60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="8"/>
+      <c r="B61" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="8"/>
+      <c r="B62" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="8"/>
+      <c r="B63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="8"/>
+      <c r="B64" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D64" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="7"/>
-      <c r="B54" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C54" s="1" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="8"/>
+      <c r="B65" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D65" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>96</v>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="8"/>
+      <c r="B68" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="8"/>
+      <c r="B69" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" s="8"/>
+      <c r="B70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" s="8"/>
+      <c r="B71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" s="8"/>
+      <c r="B72" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" s="8"/>
+      <c r="B73" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" s="8"/>
+      <c r="B74" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" s="8"/>
+      <c r="B75" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" s="8"/>
+      <c r="B76" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="A67:A76"/>
     <mergeCell ref="A23:A32"/>
     <mergeCell ref="A34:A43"/>
     <mergeCell ref="A45:A54"/>
+    <mergeCell ref="A56:A65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>